<commit_message>
add plot for BPnumber and BPlocation evaluation
</commit_message>
<xml_diff>
--- a/decomposition/tradeoff.xlsx
+++ b/decomposition/tradeoff.xlsx
@@ -354,7 +354,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -379,149 +379,160 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>93234</v>
+        <v>55986</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3">
-        <v>0.03968122285439411</v>
+        <v>0.5339792139942064</v>
       </c>
       <c r="B3">
-        <v>0.9174906239345382</v>
+        <v>0.6539576365663322</v>
       </c>
       <c r="C3">
-        <v>99042</v>
+        <v>93234</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4">
-        <v>0.3882899596165191</v>
+        <v>0.5524714886584822</v>
       </c>
       <c r="B4">
-        <v>0.6031367200818275</v>
+        <v>0.6000000000000001</v>
       </c>
       <c r="C4">
-        <v>130482</v>
+        <v>99042</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5">
-        <v>0.4279711824709137</v>
+        <v>0.7149304061728545</v>
       </c>
       <c r="B5">
-        <v>0.5206273440163656</v>
+        <v>0.3944258639910814</v>
       </c>
       <c r="C5">
-        <v>136290</v>
+        <v>130482</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6">
-        <v>0.4377831988114507</v>
+        <v>0.7334226808371306</v>
       </c>
       <c r="B6">
-        <v>0.4587453119672691</v>
+        <v>0.3404682274247492</v>
       </c>
       <c r="C6">
-        <v>142098</v>
+        <v>136290</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7">
-        <v>0.602442912692049</v>
+        <v>0.7379952844044493</v>
       </c>
       <c r="B7">
-        <v>0.3385612001363792</v>
+        <v>0.3</v>
       </c>
       <c r="C7">
-        <v>167730</v>
+        <v>142098</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8">
-        <v>0.6421241355464431</v>
+        <v>0.8147301336905748</v>
       </c>
       <c r="B8">
-        <v>0.2560518240709172</v>
+        <v>0.2214046822742475</v>
       </c>
       <c r="C8">
-        <v>173538</v>
+        <v>167730</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9">
-        <v>0.6582737667833003</v>
+        <v>0.8332224083548506</v>
       </c>
       <c r="B9">
-        <v>0.1941697920218207</v>
+        <v>0.1674470457079153</v>
       </c>
       <c r="C9">
-        <v>179346</v>
+        <v>173538</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10">
-        <v>0.6615953712294889</v>
+        <v>0.8407484721975544</v>
       </c>
       <c r="B10">
-        <v>0.1529151039890897</v>
+        <v>0.1269788182831661</v>
       </c>
       <c r="C10">
-        <v>185154</v>
+        <v>179346</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11">
-        <v>0.9308827281239934</v>
+        <v>0.8422964089123676</v>
       </c>
       <c r="B11">
-        <v>0.1529151039890897</v>
+        <v>0.1</v>
       </c>
       <c r="C11">
-        <v>204978</v>
+        <v>185154</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12">
-        <v>0.9707578740471273</v>
+        <v>0.9677899146337673</v>
       </c>
       <c r="B12">
-        <v>0.123764064098193</v>
+        <v>0.1</v>
       </c>
       <c r="C12">
-        <v>210786</v>
+        <v>204978</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13">
-        <v>0.9867135822152447</v>
+        <v>0.9863725614789619</v>
       </c>
       <c r="B13">
-        <v>0.0618820320490965</v>
+        <v>0.08093645484949834</v>
       </c>
       <c r="C13">
-        <v>216594</v>
+        <v>210786</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14">
-        <v>0.9946130334949257</v>
+        <v>0.9938082531407469</v>
       </c>
       <c r="B14">
-        <v>0.0206273440163655</v>
+        <v>0.04046822742474917</v>
       </c>
       <c r="C14">
-        <v>222402</v>
+        <v>216594</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15">
+        <v>0.9974895616351184</v>
+      </c>
+      <c r="B15">
+        <v>0.01348940914158306</v>
+      </c>
+      <c r="C15">
+        <v>222402</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16">
         <v>1</v>
       </c>
-      <c r="B15">
+      <c r="B16">
         <v>0</v>
       </c>
-      <c r="C15">
+      <c r="C16">
         <v>228210</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update taskgroup_mnist use variety score and cost now
</commit_message>
<xml_diff>
--- a/decomposition/tradeoff.xlsx
+++ b/decomposition/tradeoff.xlsx
@@ -354,7 +354,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:C28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -373,167 +373,299 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
         <v>0</v>
       </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
       <c r="C2">
-        <v>55986</v>
+        <v>103014</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3">
-        <v>0.5339792139942064</v>
+        <v>1</v>
       </c>
       <c r="B3">
-        <v>0.6539576365663322</v>
+        <v>0.2056551268874797</v>
       </c>
       <c r="C3">
-        <v>93234</v>
+        <v>104182</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4">
-        <v>0.5524714886584822</v>
+        <v>0.7871077816753987</v>
       </c>
       <c r="B4">
-        <v>0.6000000000000001</v>
+        <v>0.2056551268874797</v>
       </c>
       <c r="C4">
-        <v>99042</v>
+        <v>144902</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5">
-        <v>0.7149304061728545</v>
+        <v>0.7871077816753987</v>
       </c>
       <c r="B5">
-        <v>0.3944258639910814</v>
+        <v>0.2953213847735023</v>
       </c>
       <c r="C5">
-        <v>130482</v>
+        <v>146070</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6">
-        <v>0.7334226808371306</v>
+        <v>0.5458078442389603</v>
       </c>
       <c r="B6">
-        <v>0.3404682274247492</v>
+        <v>0.4757323837457365</v>
       </c>
       <c r="C6">
-        <v>136290</v>
+        <v>147238</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7">
-        <v>0.7379952844044493</v>
+        <v>0.5458078442389603</v>
       </c>
       <c r="B7">
-        <v>0.3</v>
+        <v>0.4757323837457365</v>
       </c>
       <c r="C7">
-        <v>142098</v>
+        <v>186790</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8">
-        <v>0.8147301336905748</v>
+        <v>0.5458078442389603</v>
       </c>
       <c r="B8">
-        <v>0.2214046822742475</v>
+        <v>0.4757323837457365</v>
       </c>
       <c r="C8">
-        <v>167730</v>
+        <v>187958</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9">
-        <v>0.8332224083548506</v>
+        <v>0.5458078442389603</v>
       </c>
       <c r="B9">
-        <v>0.1674470457079153</v>
+        <v>0.5691517309668779</v>
       </c>
       <c r="C9">
-        <v>173538</v>
+        <v>189126</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10">
-        <v>0.8407484721975544</v>
+        <v>0.5458078442389603</v>
       </c>
       <c r="B10">
-        <v>0.1269788182831661</v>
+        <v>0.7140358456794925</v>
       </c>
       <c r="C10">
-        <v>179346</v>
+        <v>190294</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11">
-        <v>0.8422964089123676</v>
+        <v>0.5125494866107783</v>
       </c>
       <c r="B11">
-        <v>0.1</v>
+        <v>0.7140358456794925</v>
       </c>
       <c r="C11">
-        <v>185154</v>
+        <v>228678</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12">
-        <v>0.9677899146337673</v>
+        <v>0.359736017481359</v>
       </c>
       <c r="B12">
-        <v>0.1</v>
+        <v>0.7140358456794925</v>
       </c>
       <c r="C12">
-        <v>204978</v>
+        <v>229846</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13">
-        <v>0.9863725614789619</v>
+        <v>0.359736017481359</v>
       </c>
       <c r="B13">
-        <v>0.08093645484949834</v>
+        <v>0.7140358456794925</v>
       </c>
       <c r="C13">
-        <v>210786</v>
+        <v>231014</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14">
-        <v>0.9938082531407469</v>
+        <v>0.359736017481359</v>
       </c>
       <c r="B14">
-        <v>0.04046822742474917</v>
+        <v>0.7280207055893819</v>
       </c>
       <c r="C14">
-        <v>216594</v>
+        <v>232182</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15">
-        <v>0.9974895616351184</v>
+        <v>0.1620043134970038</v>
       </c>
       <c r="B15">
-        <v>0.01348940914158306</v>
+        <v>0.8252441279152454</v>
       </c>
       <c r="C15">
-        <v>222402</v>
+        <v>233350</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16">
+        <v>0.1620043134970038</v>
+      </c>
+      <c r="B16">
+        <v>0.8252441279152454</v>
+      </c>
+      <c r="C16">
+        <v>270566</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17">
+        <v>0.1620043134970038</v>
+      </c>
+      <c r="B17">
+        <v>0.8252441279152454</v>
+      </c>
+      <c r="C17">
+        <v>271734</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18">
+        <v>0.1620043134970038</v>
+      </c>
+      <c r="B18">
+        <v>0.8252441279152454</v>
+      </c>
+      <c r="C18">
+        <v>272902</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19">
+        <v>0.1620043134970038</v>
+      </c>
+      <c r="B19">
+        <v>0.8252441279152454</v>
+      </c>
+      <c r="C19">
+        <v>274070</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20">
+        <v>0.1620043134970038</v>
+      </c>
+      <c r="B20">
+        <v>0.8700772568582568</v>
+      </c>
+      <c r="C20">
+        <v>275238</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21">
+        <v>0.1020690647786086</v>
+      </c>
+      <c r="B21">
+        <v>0.9682262050754993</v>
+      </c>
+      <c r="C21">
+        <v>276406</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22">
+        <v>0.1020690647786086</v>
+      </c>
+      <c r="B22">
+        <v>0.9682262050754993</v>
+      </c>
+      <c r="C22">
+        <v>312454</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23">
+        <v>0.09408290090872004</v>
+      </c>
+      <c r="B23">
+        <v>0.9682262050754993</v>
+      </c>
+      <c r="C23">
+        <v>313622</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24">
+        <v>0.05307277450263438</v>
+      </c>
+      <c r="B24">
+        <v>0.9682262050754993</v>
+      </c>
+      <c r="C24">
+        <v>314790</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25">
+        <v>0.05307277450263438</v>
+      </c>
+      <c r="B25">
+        <v>0.9682262050754993</v>
+      </c>
+      <c r="C25">
+        <v>315958</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26">
+        <v>0.03763316036348742</v>
+      </c>
+      <c r="B26">
+        <v>0.9682262050754993</v>
+      </c>
+      <c r="C26">
+        <v>317126</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27">
+        <v>0.02246601727366483</v>
+      </c>
+      <c r="B27">
+        <v>0.9682262050754993</v>
+      </c>
+      <c r="C27">
+        <v>318294</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28">
+        <v>0</v>
+      </c>
+      <c r="B28">
         <v>1</v>
       </c>
-      <c r="B16">
-        <v>0</v>
-      </c>
-      <c r="C16">
-        <v>228210</v>
+      <c r="C28">
+        <v>319462</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
use weighted variety score and cost to evaluate BPlocation
</commit_message>
<xml_diff>
--- a/decomposition/tradeoff.xlsx
+++ b/decomposition/tradeoff.xlsx
@@ -387,7 +387,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>0.2056551268874797</v>
+        <v>0.2056551268874796</v>
       </c>
       <c r="C3">
         <v>104182</v>
@@ -395,10 +395,10 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4">
-        <v>0.7871077816753987</v>
+        <v>1</v>
       </c>
       <c r="B4">
-        <v>0.2056551268874797</v>
+        <v>0.2056551268874796</v>
       </c>
       <c r="C4">
         <v>144902</v>
@@ -406,10 +406,10 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5">
-        <v>0.7871077816753987</v>
+        <v>0.7895487297993826</v>
       </c>
       <c r="B5">
-        <v>0.2953213847735023</v>
+        <v>0.2897172436556258</v>
       </c>
       <c r="C5">
         <v>146070</v>
@@ -417,10 +417,10 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6">
-        <v>0.5458078442389603</v>
+        <v>0.7581877628298113</v>
       </c>
       <c r="B6">
-        <v>0.4757323837457365</v>
+        <v>0.412184793896735</v>
       </c>
       <c r="C6">
         <v>147238</v>
@@ -428,10 +428,10 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7">
-        <v>0.5458078442389603</v>
+        <v>0.7581877628298113</v>
       </c>
       <c r="B7">
-        <v>0.4757323837457365</v>
+        <v>0.412184793896735</v>
       </c>
       <c r="C7">
         <v>186790</v>
@@ -439,10 +439,10 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8">
-        <v>0.5458078442389603</v>
+        <v>0.4717615158673499</v>
       </c>
       <c r="B8">
-        <v>0.4757323837457365</v>
+        <v>0.412184793896735</v>
       </c>
       <c r="C8">
         <v>187958</v>
@@ -450,10 +450,10 @@
     </row>
     <row r="9" spans="1:3">
       <c r="A9">
-        <v>0.5458078442389603</v>
+        <v>0.4717615158673499</v>
       </c>
       <c r="B9">
-        <v>0.5691517309668779</v>
+        <v>0.4953213847735023</v>
       </c>
       <c r="C9">
         <v>189126</v>
@@ -461,10 +461,10 @@
     </row>
     <row r="10" spans="1:3">
       <c r="A10">
-        <v>0.5458078442389603</v>
+        <v>0.2747328878457984</v>
       </c>
       <c r="B10">
-        <v>0.7140358456794925</v>
+        <v>0.6028275634437397</v>
       </c>
       <c r="C10">
         <v>190294</v>
@@ -472,10 +472,10 @@
     </row>
     <row r="11" spans="1:3">
       <c r="A11">
-        <v>0.5125494866107783</v>
+        <v>0.2747328878457984</v>
       </c>
       <c r="B11">
-        <v>0.7140358456794925</v>
+        <v>0.6028275634437397</v>
       </c>
       <c r="C11">
         <v>228678</v>
@@ -483,10 +483,10 @@
     </row>
     <row r="12" spans="1:3">
       <c r="A12">
-        <v>0.359736017481359</v>
+        <v>0.2747328878457984</v>
       </c>
       <c r="B12">
-        <v>0.7140358456794925</v>
+        <v>0.6028275634437397</v>
       </c>
       <c r="C12">
         <v>229846</v>
@@ -494,10 +494,10 @@
     </row>
     <row r="13" spans="1:3">
       <c r="A13">
-        <v>0.359736017481359</v>
+        <v>0.2747328878457984</v>
       </c>
       <c r="B13">
-        <v>0.7140358456794925</v>
+        <v>0.6028275634437397</v>
       </c>
       <c r="C13">
         <v>231014</v>
@@ -505,10 +505,10 @@
     </row>
     <row r="14" spans="1:3">
       <c r="A14">
-        <v>0.359736017481359</v>
+        <v>0.2747328878457984</v>
       </c>
       <c r="B14">
-        <v>0.7280207055893819</v>
+        <v>0.6588689746225038</v>
       </c>
       <c r="C14">
         <v>232182</v>
@@ -516,10 +516,10 @@
     </row>
     <row r="15" spans="1:3">
       <c r="A15">
-        <v>0.1620043134970038</v>
+        <v>0.2747328878457984</v>
       </c>
       <c r="B15">
-        <v>0.8252441279152454</v>
+        <v>0.777583435528494</v>
       </c>
       <c r="C15">
         <v>233350</v>
@@ -527,10 +527,10 @@
     </row>
     <row r="16" spans="1:3">
       <c r="A16">
-        <v>0.1620043134970038</v>
+        <v>0.2747328878457984</v>
       </c>
       <c r="B16">
-        <v>0.8252441279152454</v>
+        <v>0.777583435528494</v>
       </c>
       <c r="C16">
         <v>270566</v>
@@ -538,10 +538,10 @@
     </row>
     <row r="17" spans="1:3">
       <c r="A17">
-        <v>0.1620043134970038</v>
+        <v>0.2747328878457984</v>
       </c>
       <c r="B17">
-        <v>0.8252441279152454</v>
+        <v>0.777583435528494</v>
       </c>
       <c r="C17">
         <v>271734</v>
@@ -549,10 +549,10 @@
     </row>
     <row r="18" spans="1:3">
       <c r="A18">
-        <v>0.1620043134970038</v>
+        <v>0.1802214320095873</v>
       </c>
       <c r="B18">
-        <v>0.8252441279152454</v>
+        <v>0.777583435528494</v>
       </c>
       <c r="C18">
         <v>272902</v>
@@ -560,10 +560,10 @@
     </row>
     <row r="19" spans="1:3">
       <c r="A19">
-        <v>0.1620043134970038</v>
+        <v>0.1454277624071335</v>
       </c>
       <c r="B19">
-        <v>0.8252441279152454</v>
+        <v>0.777583435528494</v>
       </c>
       <c r="C19">
         <v>274070</v>
@@ -571,10 +571,10 @@
     </row>
     <row r="20" spans="1:3">
       <c r="A20">
-        <v>0.1620043134970038</v>
+        <v>0.1454277624071335</v>
       </c>
       <c r="B20">
-        <v>0.8700772568582568</v>
+        <v>0.816812423353629</v>
       </c>
       <c r="C20">
         <v>275238</v>
@@ -582,10 +582,10 @@
     </row>
     <row r="21" spans="1:3">
       <c r="A21">
-        <v>0.1020690647786086</v>
+        <v>0.06537097058055127</v>
       </c>
       <c r="B21">
-        <v>0.9682262050754993</v>
+        <v>0.8887917177642474</v>
       </c>
       <c r="C21">
         <v>276406</v>
@@ -593,10 +593,10 @@
     </row>
     <row r="22" spans="1:3">
       <c r="A22">
-        <v>0.1020690647786086</v>
+        <v>0.06537097058055127</v>
       </c>
       <c r="B22">
-        <v>0.9682262050754993</v>
+        <v>0.8887917177642474</v>
       </c>
       <c r="C22">
         <v>312454</v>
@@ -604,10 +604,10 @@
     </row>
     <row r="23" spans="1:3">
       <c r="A23">
-        <v>0.09408290090872004</v>
+        <v>0.06537097058055127</v>
       </c>
       <c r="B23">
-        <v>0.9682262050754993</v>
+        <v>0.8887917177642474</v>
       </c>
       <c r="C23">
         <v>313622</v>
@@ -615,10 +615,10 @@
     </row>
     <row r="24" spans="1:3">
       <c r="A24">
-        <v>0.05307277450263438</v>
+        <v>0.06272193393914718</v>
       </c>
       <c r="B24">
-        <v>0.9682262050754993</v>
+        <v>0.8887917177642474</v>
       </c>
       <c r="C24">
         <v>314790</v>
@@ -626,10 +626,10 @@
     </row>
     <row r="25" spans="1:3">
       <c r="A25">
-        <v>0.05307277450263438</v>
+        <v>0.04006855027803726</v>
       </c>
       <c r="B25">
-        <v>0.9682262050754993</v>
+        <v>0.8887917177642474</v>
       </c>
       <c r="C25">
         <v>315958</v>
@@ -637,10 +637,10 @@
     </row>
     <row r="26" spans="1:3">
       <c r="A26">
-        <v>0.03763316036348742</v>
+        <v>0.03169260266964554</v>
       </c>
       <c r="B26">
-        <v>0.9682262050754993</v>
+        <v>0.8887917177642474</v>
       </c>
       <c r="C26">
         <v>317126</v>
@@ -648,10 +648,10 @@
     </row>
     <row r="27" spans="1:3">
       <c r="A27">
-        <v>0.02246601727366483</v>
+        <v>0.01644936305047768</v>
       </c>
       <c r="B27">
-        <v>0.9682262050754993</v>
+        <v>0.958868974622504</v>
       </c>
       <c r="C27">
         <v>318294</v>

</xml_diff>